<commit_message>
fix: bot almost finished
</commit_message>
<xml_diff>
--- a/MID/Create-Set/Data.xlsx
+++ b/MID/Create-Set/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\MID\Create-Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF7907B4-599A-4D8F-B859-5F81306FDEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8B2F8D-B4A0-47E5-B65A-CB4B700C6EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA559316-2AF9-4D0B-B5C6-461FA99B0A82}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>4718301460</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -597,7 +597,7 @@
         <v>4718301303</v>
       </c>
       <c r="B5" s="2">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
@@ -817,5 +817,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>